<commit_message>
Output sample file now copying safely. Excel app opens/close on file read/save operations. Excel process killing after file operations. Error in Get_VariantDetailsList() function fixed.
</commit_message>
<xml_diff>
--- a/research/123.xlsx
+++ b/research/123.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Пустой выходной шаблон" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="61">
   <si>
     <t>НСО-8-10/11,1К(К-12)</t>
   </si>
@@ -197,7 +198,19 @@
     <t>ШКОС-Л -1U/2 -48 -LC ~48 -LC/SM ~48 -LC/UPC</t>
   </si>
   <si>
-    <t>и тд</t>
+    <t>1. Кабельная продукция</t>
+  </si>
+  <si>
+    <t>2. Кроссовое оборудование</t>
+  </si>
+  <si>
+    <t>3. Кабельная арматура</t>
+  </si>
+  <si>
+    <t>4.Прочие материалы</t>
+  </si>
+  <si>
+    <t>Муфта оптическая</t>
   </si>
 </sst>
 </file>
@@ -274,9 +287,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +295,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
@@ -705,10 +718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,23 +734,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
@@ -1054,280 +1067,371 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2">
         <v>5</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H23" s="1">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="3">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="3">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="2">
         <v>5</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H30" s="1">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>56</v>
-      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1339,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C5" activeCellId="1" sqref="B5 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,266 +1462,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1627,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B19:B20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,66 +1776,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>